<commit_message>
Modification of the column name
</commit_message>
<xml_diff>
--- a/master-thesis-2020/data.xlsx
+++ b/master-thesis-2020/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solen\OneDrive\Bureau\Imperial\Master project\Data analysis project\datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solen\msc-2020-bioMedEng\master-thesis-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{AC6EB9FF-C769-42F6-9628-D980A82F939F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9EB9993F-F4DD-4D93-98BF-EA29901E8BF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB4DA5B-132B-4670-B405-311FCB643C80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9ECDA5BA-65F3-4C6F-BE60-2DE617ABC656}"/>
+    <workbookView xWindow="1044" yWindow="1044" windowWidth="17280" windowHeight="8964" xr2:uid="{9ECDA5BA-65F3-4C6F-BE60-2DE617ABC656}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>Post ESCIT Basal</t>
+    <t>Post</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Post ESCIT Basal</c:v>
+                  <c:v>Post</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4914,7 +4914,7 @@
   <dimension ref="A1:C301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>